<commit_message>
capitlization edits to figure
</commit_message>
<xml_diff>
--- a/constrained_optimization/atus.xlsx
+++ b/constrained_optimization/atus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrietbrookesgray/Dropbox/My Mac (Harriets-Air.fios-router.home)/Documents/GitHub/bfh-textbook/constrained_optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A691B0-5B3E-C74C-BE15-344BDCFC9930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D80FDE-F11E-0B4C-8E30-5CE344412FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{890B4481-F0C2-1E47-9FFB-143ACFC6D781}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>Care work</t>
   </si>
   <si>
-    <t>Paid Work</t>
-  </si>
-  <si>
     <t>Personal care</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Leisure &amp; sports</t>
+  </si>
+  <si>
+    <t>Paid work</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <f>8.88-B3</f>
@@ -477,7 +477,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>1.23</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>6.43</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.27</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>3.97</v>

</xml_diff>